<commit_message>
Birth corr & morrate corr & report
</commit_message>
<xml_diff>
--- a/popsize/birthrate.xlsx
+++ b/popsize/birthrate.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Cohort</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>avg births on 1000 female (year)</t>
+  </si>
+  <si>
+    <t>avg%</t>
   </si>
 </sst>
 </file>
@@ -366,103 +369,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>26.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <f>ABS(B2/1000)</f>
+        <v>2.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>87.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C8" si="0">ABS(B3/1000)</f>
+        <v>8.7499999999999994E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>99.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>9.98E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>68.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.8199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>31.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>